<commit_message>
Added RGB Panel board.
*. Updated RS232 board
*. Minor fix in BOM fort the 8x pixel board
</commit_message>
<xml_diff>
--- a/eagle/Orange-Pi-Zero/Pixel8x/P4/BOM.xlsx
+++ b/eagle/Orange-Pi-Zero/Pixel8x/P4/BOM.xlsx
@@ -109,7 +109,7 @@
     <t xml:space="preserve">https://www.digikey.nl/product-detail/nl/kemet/C0603C104K8RACTU/399-1095-1-ND/411370</t>
   </si>
   <si>
-    <t xml:space="preserve">C13, C14 </t>
+    <t xml:space="preserve">C12, C13</t>
   </si>
   <si>
     <t xml:space="preserve">C0805C106K8PACTU</t>
@@ -628,9 +628,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>776880</xdr:colOff>
+      <xdr:colOff>776520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>186840</xdr:rowOff>
+      <xdr:rowOff>186480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -644,7 +644,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="360" y="0"/>
-          <a:ext cx="1351800" cy="372600"/>
+          <a:ext cx="1350720" cy="372240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -667,13 +667,13 @@
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="4.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.21"/>

</xml_diff>